<commit_message>
basename parameter  - "posta"
</commit_message>
<xml_diff>
--- a/output/web/reports/osm_utcanev_export.xlsx
+++ b/output/web/reports/osm_utcanev_export.xlsx
@@ -33,10 +33,10 @@
     <t>_db_nincs_hasonlo_osm</t>
   </si>
   <si>
-    <t>_db_valasztasi</t>
-  </si>
-  <si>
-    <t>_db_nincs_hasonlo_val</t>
+    <t>_db_bazis</t>
+  </si>
+  <si>
+    <t>_db_nincs_hasonlo_baz</t>
   </si>
   <si>
     <t>Debrecen</t>
@@ -11340,7 +11340,7 @@
         <v>0</v>
       </c>
       <c r="G89" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90">
@@ -24151,7 +24151,7 @@
         <v>0</v>
       </c>
       <c r="G646" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="647">
@@ -32224,7 +32224,7 @@
         <v>0</v>
       </c>
       <c r="G997" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="998">
@@ -43494,7 +43494,7 @@
         <v>0</v>
       </c>
       <c r="G1487" s="2">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="1488">
@@ -55155,7 +55155,7 @@
         <v>0</v>
       </c>
       <c r="G1994" s="2">
-        <v>1417</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1995">
@@ -59962,7 +59962,7 @@
         <v>0</v>
       </c>
       <c r="G2203" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2204">

</xml_diff>